<commit_message>
Made some nicer formatting.
</commit_message>
<xml_diff>
--- a/public/assets/data/third_party_scenarios.xlsx
+++ b/public/assets/data/third_party_scenarios.xlsx
@@ -2395,7 +2395,7 @@
       <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.1640625" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0"/>
@@ -2464,18 +2464,18 @@
         <v>4</v>
       </c>
       <c r="D3" s="11">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E3" s="11">
-        <v>0.64</v>
+        <v>0.6</v>
       </c>
       <c r="F3" s="13">
         <f>SUM(Table1[adjusted_electors_clinton])</f>
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="G3" s="32" t="str">
         <f>U63</f>
-        <v>Michigan,Pennsylvania,Wisconsin</v>
+        <v>Michigan,Wisconsin</v>
       </c>
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
@@ -2511,15 +2511,15 @@
       </c>
       <c r="D4" s="12">
         <f>1-pct_stein_to_clinton</f>
-        <v>0.19999999999999996</v>
+        <v>9.9999999999999978E-2</v>
       </c>
       <c r="E4" s="12">
         <f>1-pct_johnson_to_clinton</f>
-        <v>0.36</v>
+        <v>0.4</v>
       </c>
       <c r="F4" s="13">
         <f>SUM(Table1[adjusted_electors_trump])</f>
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="G4" s="32" t="str">
         <f>V63</f>
@@ -2701,23 +2701,23 @@
       </c>
       <c r="L11" s="31">
         <f t="shared" si="0"/>
-        <v>63781071.120000012</v>
+        <v>63734574.599999994</v>
       </c>
       <c r="M11" s="31">
         <f t="shared" si="0"/>
-        <v>61628198.880000003</v>
+        <v>61674695.400000006</v>
       </c>
       <c r="N11" s="31">
         <f t="shared" si="0"/>
-        <v>-2152872.240000003</v>
+        <v>-2059879.1999999993</v>
       </c>
       <c r="O11" s="31">
         <f t="shared" si="0"/>
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="P11" s="31">
         <f t="shared" si="0"/>
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="Q11" s="21"/>
       <c r="R11" s="21"/>
@@ -2834,15 +2834,15 @@
       </c>
       <c r="L13" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>753589.76000000001</v>
+        <v>752763.70000000007</v>
       </c>
       <c r="M13" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>1324575.24</v>
+        <v>1325401.3</v>
       </c>
       <c r="N13" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>570985.48</v>
+        <v>572637.6</v>
       </c>
       <c r="O13" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -2919,15 +2919,15 @@
       </c>
       <c r="L14" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>104823.56</v>
+        <v>104682</v>
       </c>
       <c r="M14" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>135893.44</v>
+        <v>136035</v>
       </c>
       <c r="N14" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>31069.880000000005</v>
+        <v>31353</v>
       </c>
       <c r="O14" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -3004,15 +3004,15 @@
       </c>
       <c r="L15" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>955384.08</v>
+        <v>954750.5</v>
       </c>
       <c r="M15" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>1004668.92</v>
+        <v>1005302.5</v>
       </c>
       <c r="N15" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>49284.840000000084</v>
+        <v>50552</v>
       </c>
       <c r="O15" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -3089,15 +3089,15 @@
       </c>
       <c r="L16" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>405490.12</v>
+        <v>405293.1</v>
       </c>
       <c r="M16" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>690497.88</v>
+        <v>690694.89999999991</v>
       </c>
       <c r="N16" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>285007.76</v>
+        <v>285401.79999999993</v>
       </c>
       <c r="O16" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -3174,15 +3174,15 @@
       </c>
       <c r="L17" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>5784215.4400000004</v>
+        <v>5788187.2999999998</v>
       </c>
       <c r="M17" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>3098473.56</v>
+        <v>3094501.6999999997</v>
       </c>
       <c r="N17" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-2685741.8800000004</v>
+        <v>-2693685.6</v>
       </c>
       <c r="O17" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -3259,15 +3259,15 @@
       </c>
       <c r="L18" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>1225283.04</v>
+        <v>1223496.7000000002</v>
       </c>
       <c r="M18" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>1124075.96</v>
+        <v>1125862.2999999998</v>
       </c>
       <c r="N18" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-101207.08000000007</v>
+        <v>-97634.400000000373</v>
       </c>
       <c r="O18" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -3344,15 +3344,15 @@
       </c>
       <c r="L19" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>870030.55999999994</v>
+        <v>870344.5</v>
       </c>
       <c r="M19" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>658786.44000000006</v>
+        <v>658472.5</v>
       </c>
       <c r="N19" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-211244.11999999988</v>
+        <v>-211872</v>
       </c>
       <c r="O19" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -3429,15 +3429,15 @@
       </c>
       <c r="L20" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>266299.64</v>
+        <v>266519.09999999998</v>
       </c>
       <c r="M20" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>13972.36</v>
+        <v>13752.9</v>
       </c>
       <c r="N20" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-252327.28000000003</v>
+        <v>-252766.19999999998</v>
       </c>
       <c r="O20" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -3514,15 +3514,15 @@
       </c>
       <c r="L21" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>249901.64</v>
+        <v>249921.6</v>
       </c>
       <c r="M21" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>191633.36</v>
+        <v>191613.4</v>
       </c>
       <c r="N21" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-58268.280000000028</v>
+        <v>-58308.200000000012</v>
       </c>
       <c r="O21" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -3599,15 +3599,15 @@
       </c>
       <c r="L22" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>4668804.6800000006</v>
+        <v>4666966.3</v>
       </c>
       <c r="M22" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>4692481.3199999994</v>
+        <v>4694319.7</v>
       </c>
       <c r="N22" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>23676.639999998733</v>
+        <v>27353.400000000373</v>
       </c>
       <c r="O22" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -3682,15 +3682,15 @@
       </c>
       <c r="L23" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>1916430.24</v>
+        <v>1911484.6</v>
       </c>
       <c r="M23" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>2113133.7599999998</v>
+        <v>2118079.4</v>
       </c>
       <c r="N23" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>196703.51999999979</v>
+        <v>206594.79999999981</v>
       </c>
       <c r="O23" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -3767,15 +3767,15 @@
       </c>
       <c r="L24" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>287215.95999999996</v>
+        <v>287850.7</v>
       </c>
       <c r="M24" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>137102.03999999998</v>
+        <v>136467.29999999999</v>
       </c>
       <c r="N24" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-150113.91999999998</v>
+        <v>-151383.40000000002</v>
       </c>
       <c r="O24" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -3852,15 +3852,15 @@
       </c>
       <c r="L25" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>214532.04</v>
+        <v>214248.2</v>
       </c>
       <c r="M25" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>419063.95999999996</v>
+        <v>419347.80000000005</v>
       </c>
       <c r="N25" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>204531.91999999995</v>
+        <v>205099.60000000003</v>
       </c>
       <c r="O25" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -3937,15 +3937,15 @@
       </c>
       <c r="L26" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>3167661.8400000003</v>
+        <v>3166893.4</v>
       </c>
       <c r="M26" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>2206618.1599999997</v>
+        <v>2207386.6</v>
       </c>
       <c r="N26" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-961043.68000000063</v>
+        <v>-959506.79999999981</v>
       </c>
       <c r="O26" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -4020,15 +4020,15 @@
       </c>
       <c r="L27" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>1114715.72</v>
+        <v>1109370.8</v>
       </c>
       <c r="M27" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>1603124.28</v>
+        <v>1608469.2</v>
       </c>
       <c r="N27" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>488408.56000000006</v>
+        <v>499098.39999999991</v>
       </c>
       <c r="O27" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -4105,15 +4105,15 @@
       </c>
       <c r="L28" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>696371.27999999991</v>
+        <v>695190.29999999993</v>
       </c>
       <c r="M28" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>821782.72000000009</v>
+        <v>822963.70000000007</v>
       </c>
       <c r="N28" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>125411.44000000018</v>
+        <v>127773.40000000014</v>
       </c>
       <c r="O28" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -4190,15 +4190,15 @@
       </c>
       <c r="L29" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>467281.12</v>
+        <v>467405</v>
       </c>
       <c r="M29" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>679861.88</v>
+        <v>679738</v>
       </c>
       <c r="N29" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>212580.76</v>
+        <v>212333</v>
       </c>
       <c r="O29" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -4275,15 +4275,15 @@
       </c>
       <c r="L30" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>674363.76</v>
+        <v>673605.1</v>
       </c>
       <c r="M30" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>1225074.24</v>
+        <v>1225832.9000000001</v>
       </c>
       <c r="N30" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>550710.48</v>
+        <v>552227.80000000016</v>
       </c>
       <c r="O30" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -4360,15 +4360,15 @@
       </c>
       <c r="L31" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>815037.4</v>
+        <v>814921.2</v>
       </c>
       <c r="M31" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>1194469.6000000001</v>
+        <v>1194585.8</v>
       </c>
       <c r="N31" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>379432.20000000007</v>
+        <v>379664.60000000009</v>
       </c>
       <c r="O31" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -4445,15 +4445,15 @@
       </c>
       <c r="L32" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>387739.72</v>
+        <v>387637.2</v>
       </c>
       <c r="M32" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>348920.28</v>
+        <v>349022.8</v>
       </c>
       <c r="N32" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-38819.439999999944</v>
+        <v>-38614.400000000023</v>
       </c>
       <c r="O32" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -4530,15 +4530,15 @@
       </c>
       <c r="L33" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>1568930.68</v>
+        <v>1569270.3</v>
       </c>
       <c r="M33" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>905612.32000000007</v>
+        <v>905272.70000000007</v>
       </c>
       <c r="N33" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-663318.35999999987</v>
+        <v>-663997.6</v>
       </c>
       <c r="O33" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -4615,15 +4615,15 @@
       </c>
       <c r="L34" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>1568930.68</v>
+        <v>1569270.3</v>
       </c>
       <c r="M34" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>905612.32000000007</v>
+        <v>905272.70000000007</v>
       </c>
       <c r="N34" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-663318.35999999987</v>
+        <v>-663997.6</v>
       </c>
       <c r="O34" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -4700,15 +4700,15 @@
       </c>
       <c r="L35" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>2418655.2399999998</v>
+        <v>2416803</v>
       </c>
       <c r="M35" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>2351634.7600000002</v>
+        <v>2353487</v>
       </c>
       <c r="N35" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-67020.479999999516</v>
+        <v>-63316</v>
       </c>
       <c r="O35" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -4785,15 +4785,15 @@
       </c>
       <c r="L36" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>1465781.72</v>
+        <v>1464962.7</v>
       </c>
       <c r="M36" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>1369104.28</v>
+        <v>1369923.3</v>
       </c>
       <c r="N36" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-96677.439999999944</v>
+        <v>-95039.399999999907</v>
       </c>
       <c r="O36" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -4870,15 +4870,15 @@
       </c>
       <c r="L37" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>473968.88</v>
+        <v>473775.7</v>
       </c>
       <c r="M37" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>683475.12</v>
+        <v>683668.3</v>
       </c>
       <c r="N37" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>209506.24</v>
+        <v>209892.60000000003</v>
       </c>
       <c r="O37" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -4955,15 +4955,15 @@
       </c>
       <c r="L38" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>1136656.3600000001</v>
+        <v>1135308.7999999998</v>
       </c>
       <c r="M38" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>1625475.64</v>
+        <v>1626823.2000000002</v>
       </c>
       <c r="N38" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>488819.2799999998</v>
+        <v>491514.40000000037</v>
       </c>
       <c r="O38" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -5040,15 +5040,15 @@
       </c>
       <c r="L39" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>197772.52000000002</v>
+        <v>197450.4</v>
       </c>
       <c r="M39" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>285014.48</v>
+        <v>285336.60000000003</v>
       </c>
       <c r="N39" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>87241.959999999963</v>
+        <v>87886.200000000041</v>
       </c>
       <c r="O39" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -5125,15 +5125,15 @@
       </c>
       <c r="L40" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>197772.52000000002</v>
+        <v>197450.4</v>
       </c>
       <c r="M40" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>285014.48</v>
+        <v>285336.60000000003</v>
       </c>
       <c r="N40" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>87241.959999999963</v>
+        <v>87886.200000000041</v>
       </c>
       <c r="O40" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -5208,15 +5208,15 @@
       </c>
       <c r="L41" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>561624.36</v>
+        <v>560132.4</v>
       </c>
       <c r="M41" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>524746.64</v>
+        <v>526238.6</v>
       </c>
       <c r="N41" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-36877.719999999972</v>
+        <v>-33893.800000000047</v>
       </c>
       <c r="O41" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -5293,15 +5293,15 @@
       </c>
       <c r="L42" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>371348</v>
+        <v>370754.5</v>
       </c>
       <c r="M42" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>357612</v>
+        <v>358205.5</v>
       </c>
       <c r="N42" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-13736</v>
+        <v>-12549</v>
       </c>
       <c r="O42" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -5378,15 +5378,15 @@
       </c>
       <c r="L43" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>2051383.2</v>
+        <v>2052232.7</v>
       </c>
       <c r="M43" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>1548322.8</v>
+        <v>1547473.3</v>
       </c>
       <c r="N43" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-503060.39999999991</v>
+        <v>-504759.39999999991</v>
       </c>
       <c r="O43" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -5463,15 +5463,15 @@
       </c>
       <c r="L44" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>435655.36</v>
+        <v>433681.5</v>
       </c>
       <c r="M44" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>344341.64</v>
+        <v>346315.5</v>
       </c>
       <c r="N44" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-91313.719999999972</v>
+        <v>-87366</v>
       </c>
       <c r="O44" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -5548,15 +5548,15 @@
       </c>
       <c r="L45" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>4327033.4800000004</v>
+        <v>4330547.2000000002</v>
       </c>
       <c r="M45" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>2715922.52</v>
+        <v>2712408.8</v>
       </c>
       <c r="N45" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-1611110.9600000004</v>
+        <v>-1618138.4000000004</v>
       </c>
       <c r="O45" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -5631,15 +5631,15 @@
       </c>
       <c r="L46" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>2243862.16</v>
+        <v>2238750.4</v>
       </c>
       <c r="M46" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>2385608.84</v>
+        <v>2390720.6</v>
       </c>
       <c r="N46" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>141746.6799999997</v>
+        <v>151970.20000000019</v>
       </c>
       <c r="O46" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -5716,15 +5716,15 @@
       </c>
       <c r="L47" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>110205.84</v>
+        <v>109728.70000000001</v>
       </c>
       <c r="M47" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>224573.15999999997</v>
+        <v>225050.3</v>
       </c>
       <c r="N47" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>114367.31999999998</v>
+        <v>115321.59999999998</v>
       </c>
       <c r="O47" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -5801,15 +5801,15 @@
       </c>
       <c r="L48" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>2460352.36</v>
+        <v>2458039.4</v>
       </c>
       <c r="M48" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>2841541.64</v>
+        <v>2843854.6</v>
       </c>
       <c r="N48" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>381189.28000000026</v>
+        <v>385815.20000000019</v>
       </c>
       <c r="O48" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -5884,15 +5884,15 @@
       </c>
       <c r="L49" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>473121.76</v>
+        <v>469788.4</v>
       </c>
       <c r="M49" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>977934.24</v>
+        <v>981267.6</v>
       </c>
       <c r="N49" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>504812.48</v>
+        <v>511479.19999999995</v>
       </c>
       <c r="O49" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -5969,15 +5969,15 @@
       </c>
       <c r="L50" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>1025972.44</v>
+        <v>1027033.4</v>
       </c>
       <c r="M50" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>782602.56</v>
+        <v>781541.6</v>
       </c>
       <c r="N50" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-243369.87999999989</v>
+        <v>-245491.80000000005</v>
       </c>
       <c r="O50" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -6054,23 +6054,23 @@
       </c>
       <c r="L51" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>2975132.52</v>
+        <v>2974317.5999999996</v>
       </c>
       <c r="M51" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>2974078.48</v>
+        <v>2974893.4000000004</v>
       </c>
       <c r="N51" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-1054.0400000000373</v>
+        <v>575.80000000074506</v>
       </c>
       <c r="O51" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P51" s="14">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],Table1[[#This Row],[electoral_votes]],0)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q51" s="15" t="str">
         <f>IF(Table1[[#This Row],[orig_spread]]&gt;0,"Trump","Clinton")</f>
@@ -6078,11 +6078,11 @@
       </c>
       <c r="R51" s="15" t="str">
         <f>IF(Table1[[#This Row],[adjusted_spread]]&gt;0,"Trump","Clinton")</f>
-        <v>Clinton</v>
+        <v>Trump</v>
       </c>
       <c r="S51" s="14" t="b">
         <f>AND(Table1[[#This Row],[orig_outcome]]="Trump",Table1[[#This Row],[adjusted_outcome]]="Clinton")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T51" s="14" t="b">
         <f>AND(Table1[[#This Row],[orig_outcome]]="Clinton",Table1[[#This Row],[adjusted_outcome]]="Trump")</f>
@@ -6090,7 +6090,7 @@
       </c>
       <c r="U51" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_clinton]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_clinton]],CONCATENATE(U50,IF(U50="","",","),Table1[[#This Row],[State]]),U50))</f>
-        <v>Michigan,Pennsylvania</v>
+        <v>Michigan</v>
       </c>
       <c r="V51" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_trump]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_trump]],CONCATENATE(V50,IF(V40="","",","),Table1[[#This Row],[State]]),V50))</f>
@@ -6139,15 +6139,15 @@
       </c>
       <c r="L52" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>1025972.44</v>
+        <v>1027033.4</v>
       </c>
       <c r="M52" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>782602.56</v>
+        <v>781541.6</v>
       </c>
       <c r="N52" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-243369.87999999989</v>
+        <v>-245491.80000000005</v>
       </c>
       <c r="O52" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -6175,7 +6175,7 @@
       </c>
       <c r="U52" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_clinton]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_clinton]],CONCATENATE(U51,IF(U51="","",","),Table1[[#This Row],[State]]),U51))</f>
-        <v>Michigan,Pennsylvania</v>
+        <v>Michigan</v>
       </c>
       <c r="V52" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_trump]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_trump]],CONCATENATE(V51,IF(V41="","",","),Table1[[#This Row],[State]]),V51))</f>
@@ -6224,15 +6224,15 @@
       </c>
       <c r="L53" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>890980.2</v>
+        <v>890323.3</v>
       </c>
       <c r="M53" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>1163731.7999999998</v>
+        <v>1164388.7</v>
       </c>
       <c r="N53" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>272751.59999999986</v>
+        <v>274065.39999999991</v>
       </c>
       <c r="O53" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -6260,7 +6260,7 @@
       </c>
       <c r="U53" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_clinton]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_clinton]],CONCATENATE(U52,IF(U52="","",","),Table1[[#This Row],[State]]),U52))</f>
-        <v>Michigan,Pennsylvania</v>
+        <v>Michigan</v>
       </c>
       <c r="V53" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_trump]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_trump]],CONCATENATE(V52,IF(V42="","",","),Table1[[#This Row],[State]]),V52))</f>
@@ -6307,15 +6307,15 @@
       </c>
       <c r="L54" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>130782.8</v>
+        <v>129949</v>
       </c>
       <c r="M54" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>235205.2</v>
+        <v>236039</v>
       </c>
       <c r="N54" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>104422.40000000001</v>
+        <v>106090</v>
       </c>
       <c r="O54" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -6343,7 +6343,7 @@
       </c>
       <c r="U54" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_clinton]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_clinton]],CONCATENATE(U53,IF(U53="","",","),Table1[[#This Row],[State]]),U53))</f>
-        <v>Michigan,Pennsylvania</v>
+        <v>Michigan</v>
       </c>
       <c r="V54" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_trump]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_trump]],CONCATENATE(V53,IF(V43="","",","),Table1[[#This Row],[State]]),V53))</f>
@@ -6392,15 +6392,15 @@
       </c>
       <c r="L55" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>924698.96</v>
+        <v>923487.5</v>
       </c>
       <c r="M55" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>1545816.04</v>
+        <v>1547027.5</v>
       </c>
       <c r="N55" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>621117.08000000007</v>
+        <v>623540</v>
       </c>
       <c r="O55" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -6428,7 +6428,7 @@
       </c>
       <c r="U55" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_clinton]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_clinton]],CONCATENATE(U54,IF(U54="","",","),Table1[[#This Row],[State]]),U54))</f>
-        <v>Michigan,Pennsylvania</v>
+        <v>Michigan</v>
       </c>
       <c r="V55" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_trump]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_trump]],CONCATENATE(V54,IF(V44="","",","),Table1[[#This Row],[State]]),V54))</f>
@@ -6477,15 +6477,15 @@
       </c>
       <c r="L56" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>4105676.96</v>
+        <v>4101506.6999999997</v>
       </c>
       <c r="M56" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>4797560.04</v>
+        <v>4801730.3</v>
       </c>
       <c r="N56" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>691883.08000000007</v>
+        <v>700223.60000000009</v>
       </c>
       <c r="O56" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -6513,7 +6513,7 @@
       </c>
       <c r="U56" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_clinton]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_clinton]],CONCATENATE(U55,IF(U55="","",","),Table1[[#This Row],[State]]),U55))</f>
-        <v>Michigan,Pennsylvania</v>
+        <v>Michigan</v>
       </c>
       <c r="V56" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_trump]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_trump]],CONCATENATE(V55,IF(V45="","",","),Table1[[#This Row],[State]]),V55))</f>
@@ -6562,15 +6562,15 @@
       </c>
       <c r="L57" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>369874.32</v>
+        <v>361508.4</v>
       </c>
       <c r="M57" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>456331.68</v>
+        <v>464697.60000000003</v>
       </c>
       <c r="N57" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>86457.359999999986</v>
+        <v>103189.20000000001</v>
       </c>
       <c r="O57" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -6598,7 +6598,7 @@
       </c>
       <c r="U57" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_clinton]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_clinton]],CONCATENATE(U56,IF(U56="","",","),Table1[[#This Row],[State]]),U56))</f>
-        <v>Michigan,Pennsylvania</v>
+        <v>Michigan</v>
       </c>
       <c r="V57" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_trump]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_trump]],CONCATENATE(V56,IF(V46="","",","),Table1[[#This Row],[State]]),V56))</f>
@@ -6647,15 +6647,15 @@
       </c>
       <c r="L58" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>189891.84</v>
+        <v>190164.4</v>
       </c>
       <c r="M58" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>99990.159999999989</v>
+        <v>99717.599999999991</v>
       </c>
       <c r="N58" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-89901.680000000008</v>
+        <v>-90446.8</v>
       </c>
       <c r="O58" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -6683,7 +6683,7 @@
       </c>
       <c r="U58" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_clinton]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_clinton]],CONCATENATE(U57,IF(U57="","",","),Table1[[#This Row],[State]]),U57))</f>
-        <v>Michigan,Pennsylvania</v>
+        <v>Michigan</v>
       </c>
       <c r="V58" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_trump]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_trump]],CONCATENATE(V57,IF(V47="","",","),Table1[[#This Row],[State]]),V57))</f>
@@ -6732,15 +6732,15 @@
       </c>
       <c r="L59" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>2013286.6</v>
+        <v>2011349.8</v>
       </c>
       <c r="M59" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>1778586.4</v>
+        <v>1780523.2</v>
       </c>
       <c r="N59" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-234700.20000000019</v>
+        <v>-230826.60000000009</v>
       </c>
       <c r="O59" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -6768,7 +6768,7 @@
       </c>
       <c r="U59" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_clinton]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_clinton]],CONCATENATE(U58,IF(U58="","",","),Table1[[#This Row],[State]]),U58))</f>
-        <v>Michigan,Pennsylvania</v>
+        <v>Michigan</v>
       </c>
       <c r="V59" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_trump]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_trump]],CONCATENATE(V58,IF(V48="","",","),Table1[[#This Row],[State]]),V58))</f>
@@ -6817,15 +6817,15 @@
       </c>
       <c r="L60" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>1290549.72</v>
+        <v>1289949.2</v>
       </c>
       <c r="M60" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>866417.27999999991</v>
+        <v>867017.79999999993</v>
       </c>
       <c r="N60" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-424132.44000000006</v>
+        <v>-422931.4</v>
       </c>
       <c r="O60" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -6853,7 +6853,7 @@
       </c>
       <c r="U60" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_clinton]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_clinton]],CONCATENATE(U59,IF(U59="","",","),Table1[[#This Row],[State]]),U59))</f>
-        <v>Michigan,Pennsylvania</v>
+        <v>Michigan</v>
       </c>
       <c r="V60" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_trump]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_trump]],CONCATENATE(V59,IF(V49="","",","),Table1[[#This Row],[State]]),V59))</f>
@@ -6902,15 +6902,15 @@
       </c>
       <c r="L61" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>208447.72</v>
+        <v>208335.8</v>
       </c>
       <c r="M61" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>496005.28</v>
+        <v>496117.2</v>
       </c>
       <c r="N61" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>287557.56000000006</v>
+        <v>287781.40000000002</v>
       </c>
       <c r="O61" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -6938,7 +6938,7 @@
       </c>
       <c r="U61" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_clinton]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_clinton]],CONCATENATE(U60,IF(U60="","",","),Table1[[#This Row],[State]]),U60))</f>
-        <v>Michigan,Pennsylvania</v>
+        <v>Michigan</v>
       </c>
       <c r="V61" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_trump]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_trump]],CONCATENATE(V60,IF(V50="","",","),Table1[[#This Row],[State]]),V60))</f>
@@ -6987,15 +6987,15 @@
       </c>
       <c r="L62" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>1475116.88</v>
+        <v>1473957.2</v>
       </c>
       <c r="M62" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>1453982.12</v>
+        <v>1455141.8</v>
       </c>
       <c r="N62" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>-21134.759999999776</v>
+        <v>-18815.399999999907</v>
       </c>
       <c r="O62" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -7023,7 +7023,7 @@
       </c>
       <c r="U62" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_clinton]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_clinton]],CONCATENATE(U61,IF(U61="","",","),Table1[[#This Row],[State]]),U61))</f>
-        <v>Michigan,Pennsylvania,Wisconsin</v>
+        <v>Michigan,Wisconsin</v>
       </c>
       <c r="V62" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_trump]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_trump]],CONCATENATE(V61,IF(V51="","",","),Table1[[#This Row],[State]]),V61))</f>
@@ -7072,15 +7072,15 @@
       </c>
       <c r="L63" s="14">
         <f>Table1[[#This Row],[orig_vote_clinton]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_clinton+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_clinton</f>
-        <v>66461</v>
+        <v>66180.800000000003</v>
       </c>
       <c r="M63" s="14">
         <f>Table1[[#This Row],[orig_vote_trump]]+Table1[[#This Row],[orig_vote_stein]]*pct_stein_to_trump+Table1[[#This Row],[orig_vote_johnson]]*pct_johnson_to_trump</f>
-        <v>179533</v>
+        <v>179813.2</v>
       </c>
       <c r="N63" s="15">
         <f>Table1[[#This Row],[adjusted_vote_trump]]-Table1[[#This Row],[adjusted_vote_clinton]]</f>
-        <v>113072</v>
+        <v>113632.40000000001</v>
       </c>
       <c r="O63" s="15">
         <f>IF(Table1[[#This Row],[adjusted_vote_clinton]]&gt;Table1[[#This Row],[adjusted_vote_trump]],0,Table1[[#This Row],[electoral_votes]])</f>
@@ -7108,7 +7108,7 @@
       </c>
       <c r="U63" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_clinton]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_clinton]],CONCATENATE(U62,IF(U62="","",","),Table1[[#This Row],[State]]),U62))</f>
-        <v>Michigan,Pennsylvania,Wisconsin</v>
+        <v>Michigan,Wisconsin</v>
       </c>
       <c r="V63" s="14" t="str">
         <f>IF(Table1[[#This Row],[index]]=1,IF(Table1[[#This Row],[pickup_trump]],Table1[[#This Row],[State]],""),IF(Table1[[#This Row],[pickup_trump]],CONCATENATE(V62,IF(V52="","",","),Table1[[#This Row],[State]]),V62))</f>

</xml_diff>